<commit_message>
added code to example notebook
</commit_message>
<xml_diff>
--- a/test_oligos.xlsx
+++ b/test_oligos.xlsx
@@ -207,7 +207,7 @@
     <t>ggt tgc agt gag ctg aga</t>
   </si>
   <si>
-    <t>5ATTTTTTTCTAATGGTTAAGTA</t>
+    <t>ATTTTTTTCTAATGGTTAAGTA</t>
   </si>
 </sst>
 </file>
@@ -284,8 +284,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3259">
+  <cellStyleXfs count="3265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3556,7 +3562,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3259">
+  <cellStyles count="3265">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5186,6 +5192,9 @@
     <cellStyle name="Followed Hyperlink" xfId="3254" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3256" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3264" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6815,6 +6824,9 @@
     <cellStyle name="Hyperlink" xfId="3253" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3255" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3263" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7151,7 +7163,7 @@
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Added text files and edits to notebook
</commit_message>
<xml_diff>
--- a/test_oligos.xlsx
+++ b/test_oligos.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Oligos Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>KH14</t>
-  </si>
-  <si>
-    <t>CATACTTACTTGGCTTGTTTGGGATAT</t>
   </si>
   <si>
     <t>TTACGCATAAACGATGACGTCA</t>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>ATTTTTTTCTAATGGTTAAGTA</t>
+  </si>
+  <si>
+    <t>AGAGGGGCTGGGAGTTGGACCCC</t>
   </si>
 </sst>
 </file>
@@ -7163,7 +7163,7 @@
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7191,7 +7191,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -7202,10 +7202,10 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7213,7 +7213,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>5</v>
@@ -7224,7 +7224,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
@@ -7235,7 +7235,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
@@ -7246,7 +7246,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -7257,10 +7257,10 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -7268,7 +7268,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>16</v>
@@ -7279,7 +7279,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>19</v>
@@ -7287,13 +7287,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -7301,10 +7301,10 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -7312,7 +7312,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>20</v>
@@ -7323,10 +7323,10 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -7334,76 +7334,76 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="150" ht="15" customHeight="1"/>
@@ -7413,7 +7413,7 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="62" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>